<commit_message>
Before chaning factorio version
</commit_message>
<xml_diff>
--- a/Roadmap.xlsx
+++ b/Roadmap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ingemras\AppData\Roaming\Factorio\mods\TheEmpiredev_0.0.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C524DD5-2C46-4B73-A05F-DFAE3584F381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDEF1B7-83B0-4D60-9479-295B0BE6C8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2970" yWindow="3300" windowWidth="21600" windowHeight="11205" xr2:uid="{8C2B6033-0141-4B28-8554-31B7B3325C7E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8C2B6033-0141-4B28-8554-31B7B3325C7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Roadmap" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="139">
   <si>
     <t>Function</t>
   </si>
@@ -428,16 +428,34 @@
     <t>Animal density world map</t>
   </si>
   <si>
+    <t>Build squad window</t>
+  </si>
+  <si>
+    <t>Sqad templates</t>
+  </si>
+  <si>
+    <t>Split select unit window from workshop</t>
+  </si>
+  <si>
+    <t>Split itemlistbuilder from storage ui</t>
+  </si>
+  <si>
+    <t>Squad queue window</t>
+  </si>
+  <si>
+    <t>Squad templates window</t>
+  </si>
+  <si>
+    <t>Squad list window</t>
+  </si>
+  <si>
+    <t>Squad window</t>
+  </si>
+  <si>
+    <t>Try to build squads every x seconds</t>
+  </si>
+  <si>
     <t>in progress</t>
-  </si>
-  <si>
-    <t>Build squad window</t>
-  </si>
-  <si>
-    <t>Sqad templates</t>
-  </si>
-  <si>
-    <t>Split select unit window from workshop</t>
   </si>
 </sst>
 </file>
@@ -1953,20 +1971,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B25D95-7349-4075-99CF-A76FE5E9CDFC}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1977,7 +1995,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1985,7 +2003,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1993,7 +2011,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2001,7 +2019,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2009,7 +2027,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2017,7 +2035,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2025,7 +2043,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2033,7 +2051,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -2041,7 +2059,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -2049,7 +2067,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2057,7 +2075,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -2065,7 +2083,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2073,7 +2091,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -2081,7 +2099,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -2089,7 +2107,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -2097,7 +2115,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -2105,7 +2123,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -2113,7 +2131,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -2121,7 +2139,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -2129,7 +2147,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -2137,7 +2155,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -2145,7 +2163,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -2153,7 +2171,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2161,7 +2179,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>91</v>
       </c>
@@ -2169,7 +2187,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>92</v>
       </c>
@@ -2177,7 +2195,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>99</v>
       </c>
@@ -2185,7 +2203,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>93</v>
       </c>
@@ -2193,7 +2211,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -2201,7 +2219,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>95</v>
       </c>
@@ -2209,7 +2227,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>127</v>
       </c>
@@ -2217,7 +2235,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>128</v>
       </c>
@@ -2225,152 +2243,200 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>132</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B34" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>131</v>
-      </c>
-      <c r="B35" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>133</v>
+      </c>
+      <c r="B37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>134</v>
+      </c>
+      <c r="B38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>135</v>
+      </c>
+      <c r="B39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>136</v>
+      </c>
+      <c r="B40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>137</v>
+      </c>
+      <c r="B41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>16</v>
       </c>
-      <c r="B36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B42" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>45</v>
-      </c>
-      <c r="B37" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>13</v>
-      </c>
-      <c r="B38" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>19</v>
-      </c>
-      <c r="B40" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>23</v>
-      </c>
-      <c r="B42" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>24</v>
       </c>
       <c r="B43" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B44" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="B45" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B46" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B47" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B48" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B49" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B50" t="s">
         <v>32</v>
       </c>
     </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>29</v>
+      </c>
+      <c r="B52" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>30</v>
+      </c>
+      <c r="B53" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>27</v>
+      </c>
+      <c r="B55" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B37 B39:B1048576">
+  <conditionalFormatting sqref="B45:B1048576 B1:B43">
     <cfRule type="beginsWith" dxfId="5" priority="4" operator="beginsWith" text="done">
       <formula>LEFT(B1,LEN("done"))="done"</formula>
     </cfRule>
@@ -2381,15 +2447,15 @@
       <formula>LEFT(B1,LEN("to do"))="to do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B38">
+  <conditionalFormatting sqref="B44">
     <cfRule type="beginsWith" dxfId="2" priority="1" operator="beginsWith" text="done">
-      <formula>LEFT(B38,LEN("done"))="done"</formula>
+      <formula>LEFT(B44,LEN("done"))="done"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="2" operator="beginsWith" text="in progress">
-      <formula>LEFT(B38,LEN("in progress"))="in progress"</formula>
+      <formula>LEFT(B44,LEN("in progress"))="in progress"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="0" priority="3" operator="beginsWith" text="to do">
-      <formula>LEFT(B38,LEN("to do"))="to do"</formula>
+      <formula>LEFT(B44,LEN("to do"))="to do"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2405,15 +2471,15 @@
       <selection activeCell="A5" sqref="A5:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -2427,7 +2493,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>63</v>
       </c>
@@ -2441,7 +2507,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>32</v>
       </c>
@@ -2455,7 +2521,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2469,7 +2535,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>64</v>
       </c>
@@ -2483,7 +2549,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>127</v>
       </c>
@@ -2497,7 +2563,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>128</v>
       </c>
@@ -2524,13 +2590,13 @@
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -2538,7 +2604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -2546,7 +2612,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -2555,7 +2621,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -2563,7 +2629,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -2572,7 +2638,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -2581,7 +2647,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -2589,7 +2655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -2598,7 +2664,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>75</v>
       </c>
@@ -2607,7 +2673,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -2615,7 +2681,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>80</v>
       </c>
@@ -2623,7 +2689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>76</v>
       </c>
@@ -2632,7 +2698,7 @@
         <v>6.9314718055970184E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>79</v>
       </c>
@@ -2641,7 +2707,7 @@
         <v>0.13862943611194037</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>81</v>
       </c>
@@ -2650,227 +2716,227 @@
         <v>6.9314718055970186</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>114</v>
       </c>
@@ -2889,13 +2955,13 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>117</v>
       </c>
@@ -2903,7 +2969,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>123</v>
       </c>
@@ -2911,7 +2977,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>122</v>
       </c>
@@ -2919,7 +2985,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>126</v>
       </c>
@@ -2927,17 +2993,17 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>121</v>
       </c>
@@ -2955,9 +3021,9 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>77</v>
       </c>
@@ -2968,7 +3034,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2977,7 +3043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2986,7 +3052,7 @@
         <v>0.63092975357145742</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2995,7 +3061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3004,7 +3070,7 @@
         <v>1.2618595071429148</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3013,7 +3079,7 @@
         <v>1.4649735207179269</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3022,7 +3088,7 @@
         <v>1.6309297535714573</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3031,7 +3097,7 @@
         <v>1.7712437491614221</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3040,7 +3106,7 @@
         <v>1.8927892607143719</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3049,7 +3115,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3058,7 +3124,7 @@
         <v>2.0959032742893848</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3067,7 +3133,7 @@
         <v>2.1826583386441381</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3076,7 +3142,7 @@
         <v>2.2618595071429146</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3085,7 +3151,7 @@
         <v>2.3347175194727927</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3094,7 +3160,7 @@
         <v>2.4021735027328792</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3103,7 +3169,7 @@
         <v>2.4649735207179271</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3112,7 +3178,7 @@
         <v>2.5237190142858297</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3121,7 +3187,7 @@
         <v>2.5789019231625656</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3130,7 +3196,7 @@
         <v>2.6309297535714569</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3139,7 +3205,7 @@
         <v>2.6801438592463751</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3148,7 +3214,7 @@
         <v>2.7268330278608417</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>100</v>
       </c>
@@ -3157,7 +3223,7 @@
         <v>4.1918065485787697</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>200</v>
       </c>
@@ -3166,7 +3232,7 @@
         <v>4.8227363021502256</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>300</v>
       </c>
@@ -3175,7 +3241,7 @@
         <v>5.1918065485787688</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>400</v>
       </c>
@@ -3184,7 +3250,7 @@
         <v>5.4536660557216834</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>500</v>
       </c>
@@ -3193,7 +3259,7 @@
         <v>5.6567800692966959</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>600</v>
       </c>
@@ -3202,7 +3268,7 @@
         <v>5.8227363021502265</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>700</v>
       </c>
@@ -3211,7 +3277,7 @@
         <v>5.9630502977401907</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>800</v>
       </c>
@@ -3220,7 +3286,7 @@
         <v>6.0845958092931411</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>900</v>
       </c>
@@ -3229,7 +3295,7 @@
         <v>6.1918065485787688</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1000</v>
       </c>
@@ -3238,7 +3304,7 @@
         <v>6.2877098228681527</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1100</v>
       </c>
@@ -3247,7 +3313,7 @@
         <v>6.3744648872229064</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1200</v>
       </c>
@@ -3256,7 +3322,7 @@
         <v>6.4536660557216834</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1300</v>
       </c>
@@ -3265,7 +3331,7 @@
         <v>6.526524068051561</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1400</v>
       </c>
@@ -3274,7 +3340,7 @@
         <v>6.5939800513116484</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1500</v>
       </c>
@@ -3283,7 +3349,7 @@
         <v>6.6567800692966959</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1600</v>
       </c>
@@ -3292,7 +3358,7 @@
         <v>6.715525562864598</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1700</v>
       </c>
@@ -3301,7 +3367,7 @@
         <v>6.7707084717413339</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1800</v>
       </c>
@@ -3310,7 +3376,7 @@
         <v>6.8227363021502265</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1900</v>
       </c>
@@ -3319,7 +3385,7 @@
         <v>6.8719504078251443</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2000</v>
       </c>
@@ -3328,7 +3394,7 @@
         <v>6.9186395764396105</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>3000</v>
       </c>
@@ -3337,7 +3403,7 @@
         <v>7.2877098228681527</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>4000</v>
       </c>
@@ -3346,7 +3412,7 @@
         <v>7.5495693300110682</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>5000</v>
       </c>

</xml_diff>